<commit_message>
finaler commit vor Abgabe
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,35 +436,40 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Dauer in s</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>max Geschwindigkeit in m/s</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>max Geschwindigkeit in km/h</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>max Beschleunigung in m/s^2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>min Beschleunigung im m/s^2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>max Leistung in kW</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>max Drehmoment in Nm</t>
         </is>
@@ -476,11 +481,13 @@
           <t>idle1</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>idle1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1212</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -495,6 +502,9 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -504,26 +514,31 @@
           <t>drive1</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>drive1</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2709</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>13.33</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>47.988</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3.06</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>-2.5</v>
       </c>
-      <c r="G3" t="n">
-        <v>62.06</v>
-      </c>
       <c r="H3" t="n">
-        <v>296.22</v>
+        <v>62.11</v>
+      </c>
+      <c r="I3" t="n">
+        <v>296.48</v>
       </c>
     </row>
     <row r="4">
@@ -532,26 +547,31 @@
           <t>live1</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>live1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>3853</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>16.67</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>60.01200000000001</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>3.06</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>-2.78</v>
       </c>
-      <c r="G4" t="n">
-        <v>70.16</v>
-      </c>
       <c r="H4" t="n">
-        <v>389.17</v>
+        <v>70.22</v>
+      </c>
+      <c r="I4" t="n">
+        <v>389.5</v>
       </c>
     </row>
     <row r="5">
@@ -560,26 +580,31 @@
           <t>ufpe1</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ufpe1</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>1651</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>15</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>54</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>3.06</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>-4.44</v>
       </c>
-      <c r="G5" t="n">
-        <v>54</v>
-      </c>
       <c r="H5" t="n">
-        <v>328.73</v>
+        <v>54.04</v>
+      </c>
+      <c r="I5" t="n">
+        <v>328.97</v>
       </c>
     </row>
     <row r="6">
@@ -588,26 +613,31 @@
           <t>long1</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>long1</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>3528</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>22.5</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>81</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>3.61</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>-3.89</v>
       </c>
-      <c r="G6" t="n">
-        <v>99.75</v>
-      </c>
       <c r="H6" t="n">
-        <v>450.96</v>
+        <v>99.84999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>451.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>